<commit_message>
Update: Test Scenario excel sheet.
</commit_message>
<xml_diff>
--- a/Manual/Test-Scenario-Document/Test-Scenarios-Document.xlsx
+++ b/Manual/Test-Scenario-Document/Test-Scenarios-Document.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADARSH J. MISHRA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d09b73bd954f8bef/Desktop/Nopcommerce Project/Manual/Test-Scenario-Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02871991-CA98-4C32-BCF8-A4496BF3F069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{02871991-CA98-4C32-BCF8-A4496BF3F069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5863E023-1C4F-4FFB-BBA8-6543322071DF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="133">
   <si>
     <t>Scenario_ID</t>
   </si>
@@ -69,9 +69,6 @@
     <t>HP_TS_004</t>
   </si>
   <si>
-    <t>Verify that the search bar is visible with correct placeholder text.</t>
-  </si>
-  <si>
     <t>HP_TS_005</t>
   </si>
   <si>
@@ -105,51 +102,12 @@
     <t>HP_TS_010</t>
   </si>
   <si>
-    <t>Verify the image carousel auto-slides properly.</t>
-  </si>
-  <si>
-    <t>HP_TS_011</t>
-  </si>
-  <si>
     <t>Verify homepage components load properly on page refresh.</t>
   </si>
   <si>
-    <t>HP_TS_012</t>
-  </si>
-  <si>
     <t>Verify homepage UI layout for broken images or missing elements.</t>
   </si>
   <si>
-    <t>HP_TS_013</t>
-  </si>
-  <si>
-    <t>HP_TS_014</t>
-  </si>
-  <si>
-    <t>Verify footer links are visible and redirect correctly.</t>
-  </si>
-  <si>
-    <t>HP_TS_015</t>
-  </si>
-  <si>
-    <t>Verify homepage loads within acceptable performance time.</t>
-  </si>
-  <si>
-    <t>HP_TS_016</t>
-  </si>
-  <si>
-    <t>Verify homepage before and after login updates navigation correctly.</t>
-  </si>
-  <si>
-    <t>HP_TS_017</t>
-  </si>
-  <si>
-    <t>Verify wishlist/cart count updates when items are added.</t>
-  </si>
-  <si>
-    <t>Verify homepage page title and URL are correct.</t>
-  </si>
-  <si>
     <t>RG_TS_001</t>
   </si>
   <si>
@@ -189,9 +147,6 @@
     <t>RG_TS_007</t>
   </si>
   <si>
-    <t>Verify gender selection is optional/works correctly.</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -204,30 +159,15 @@
     <t>RG_TS_009</t>
   </si>
   <si>
-    <t>Verify registration success redirects to My Account.</t>
-  </si>
-  <si>
     <t>RG_TS_010</t>
   </si>
   <si>
-    <t>Verify error message shows for existing email.</t>
-  </si>
-  <si>
-    <t>RG_TS_011</t>
-  </si>
-  <si>
     <t>Verify company name is optional.</t>
   </si>
   <si>
-    <t>RG_TS_012</t>
-  </si>
-  <si>
     <t>Verify register button disabled without mandatory fields.</t>
   </si>
   <si>
-    <t>RG_TS_013</t>
-  </si>
-  <si>
     <t>Verify page loads within normal time.</t>
   </si>
   <si>
@@ -297,48 +237,6 @@
     <t>Verify error message for blank email.</t>
   </si>
   <si>
-    <t>LG_TS_011</t>
-  </si>
-  <si>
-    <t>Verify error message for blank password.</t>
-  </si>
-  <si>
-    <t>LG_TS_012</t>
-  </si>
-  <si>
-    <t>Verify user gets redirected to My Account after login.</t>
-  </si>
-  <si>
-    <t>LG_TS_013</t>
-  </si>
-  <si>
-    <t>LG_TS_014</t>
-  </si>
-  <si>
-    <t>Verify login rate limiting after multiple wrong attempts.</t>
-  </si>
-  <si>
-    <t>LG_TS_015</t>
-  </si>
-  <si>
-    <t>Verify browser back button after login remains logged in.</t>
-  </si>
-  <si>
-    <t>LG_TS_016</t>
-  </si>
-  <si>
-    <t>Verify password field accepts valid length.</t>
-  </si>
-  <si>
-    <t>LG_TS_017</t>
-  </si>
-  <si>
-    <t>Verify login using both lowercase/uppercase email.</t>
-  </si>
-  <si>
-    <t>Verify login page loads within acceptable performance time.</t>
-  </si>
-  <si>
     <t>WL_TS_001</t>
   </si>
   <si>
@@ -402,9 +300,6 @@
     <t>Verify clicking product redirects to detail page.</t>
   </si>
   <si>
-    <t>WL_TS_011</t>
-  </si>
-  <si>
     <t>CT_TS_001</t>
   </si>
   <si>
@@ -465,27 +360,9 @@
     <t>CT_TS_010</t>
   </si>
   <si>
-    <t>CT_TS_011</t>
-  </si>
-  <si>
     <t>Verify cart UI elements load properly.</t>
   </si>
   <si>
-    <t>CT_TS_012</t>
-  </si>
-  <si>
-    <t>Verify product images appear in cart.</t>
-  </si>
-  <si>
-    <t>CT_TS_013</t>
-  </si>
-  <si>
-    <t>Verify redirect from cart to product page via product name link.</t>
-  </si>
-  <si>
-    <t>Verify cart performs correctly on page refresh.</t>
-  </si>
-  <si>
     <t>ACC_TS_001</t>
   </si>
   <si>
@@ -547,40 +424,13 @@
   </si>
   <si>
     <t>Verify navigation links on left menu redirect properly.</t>
-  </si>
-  <si>
-    <t>ACC_TS_011</t>
-  </si>
-  <si>
-    <t>Verify addresses tab loads correctly.</t>
-  </si>
-  <si>
-    <t>ACC_TS_012</t>
-  </si>
-  <si>
-    <t>Verify orders tab loads user order history.</t>
-  </si>
-  <si>
-    <t>ACC_TS_013</t>
-  </si>
-  <si>
-    <t>Verify change password link functionality.</t>
-  </si>
-  <si>
-    <t>ACC_TS_014</t>
-  </si>
-  <si>
-    <t>Verify downloadable products tab loads correct data.</t>
-  </si>
-  <si>
-    <t>Verify user cannot wishlist without login.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,6 +442,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -658,6 +515,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -960,10 +821,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,7 +896,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -1046,77 +907,77 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>26</v>
@@ -1125,108 +986,11 @@
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1236,10 +1000,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1266,13 +1030,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -1280,13 +1044,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1294,13 +1058,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -1308,13 +1072,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -1322,13 +1086,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
@@ -1336,117 +1100,76 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1456,10 +1179,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1486,13 +1209,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -1500,13 +1223,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1514,13 +1237,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -1528,13 +1251,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
@@ -1542,13 +1265,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
@@ -1556,13 +1279,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -1570,13 +1293,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -1584,13 +1307,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
@@ -1598,13 +1321,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
@@ -1612,114 +1335,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1732,10 +1357,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1762,13 +1387,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -1776,13 +1401,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1790,13 +1415,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -1804,13 +1429,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -1818,13 +1443,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -1832,13 +1457,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -1846,13 +1471,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -1860,27 +1485,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
@@ -1888,29 +1513,15 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1924,10 +1535,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1954,13 +1565,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -1968,13 +1579,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1982,13 +1593,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -1996,13 +1607,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -2010,13 +1621,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
@@ -2024,13 +1635,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -2038,13 +1649,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -2052,13 +1663,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
@@ -2066,13 +1677,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
@@ -2080,58 +1691,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2144,10 +1713,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2174,13 +1743,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -2188,13 +1757,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>157</v>
+        <v>116</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -2202,13 +1771,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>159</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -2216,13 +1785,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -2230,27 +1799,27 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -2258,13 +1827,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -2272,13 +1841,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>168</v>
+        <v>127</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>169</v>
+        <v>128</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
@@ -2286,13 +1855,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>170</v>
+        <v>129</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
@@ -2300,72 +1869,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>